<commit_message>
Adaptação para o cloud
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colaborador\Documents\UiPath\ReporterUniversal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6599FE8-1FEC-4289-A4DB-FB007304B7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDC93BD-9088-464B-AA8A-F097728A58D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="21624" windowHeight="11112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -147,9 +147,6 @@
     <t>OR.Execution OR.Assets OR.Queues OR.Jobs OR.Users OR.Administration OR.Machines OR.License OR.Settings OR.Robots OR.Audit OR.TestSetExecutions OR.TestSetSchedules OR.TestSets OR.TestDataQueues OR.Hypervisor OR.BackgroundTasks OR.Webhooks OR.Monitoring OR.ML OR.Tasks OR.Analytics OR.Folders</t>
   </si>
   <si>
-    <t>odata/QueueItems?$top={0}&amp;$filter=QueueDefinitionId eq {1} and (Status eq 'New' or Status eq 'Successful' or Status eq 'Failed')&amp;$orderby=StartProcessing desc&amp;$skip={2}</t>
-  </si>
-  <si>
     <t>OrchestratorAppScope</t>
   </si>
   <si>
@@ -193,6 +190,15 @@
   </si>
   <si>
     <t>aroucagabriel/Desktop/odata/QueueDefinitions</t>
+  </si>
+  <si>
+    <t>OR.Assets.Read OR.Execution.Read OR.Folders.Read OR.Jobs.Read OR.Queues.Read OR.Robots.Read</t>
+  </si>
+  <si>
+    <t>PostmanScope</t>
+  </si>
+  <si>
+    <t>aroucagabriel/Desktop/odata/QueueItems?$top={0}&amp;$filter=QueueDefinitionId eq {1} and (Status eq 'New' or Status eq 'Successful' or Status eq 'Failed')&amp;$orderby=StartProcessing desc&amp;$skip={2}</t>
   </si>
 </sst>
 </file>
@@ -579,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -630,7 +636,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>22</v>
@@ -638,10 +644,10 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="C3" s="6"/>
     </row>
@@ -661,7 +667,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -669,7 +675,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -677,7 +683,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -685,7 +691,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -706,7 +712,7 @@
     </row>
     <row r="11" spans="1:26" ht="48.75" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>39</v>
@@ -714,13 +720,20 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2883,26 +2896,26 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Finalizada V1 da refatoração para CNDs
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Elera_ReporterUniversal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA419B86-BB57-47D4-9D06-E381F70F0BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C325DEF-7C2F-49CA-87B7-9CEAEBEFD12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>MailSubject</t>
+  </si>
+  <si>
+    <t>ColumnsToKeep</t>
+  </si>
+  <si>
+    <t>Empresa,CNPJ,Nível,Certidão,Data de Validade,Status,Etapa,Início</t>
   </si>
 </sst>
 </file>
@@ -600,7 +606,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -748,7 +754,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Adicionado leitura do config no storage bucket
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Elera_ReporterUniversal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C325DEF-7C2F-49CA-87B7-9CEAEBEFD12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415B3615-828A-498B-9D1A-5D2F37C7FFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -186,21 +186,12 @@
     <t>Orchestrator_AppClientIdAndSecret</t>
   </si>
   <si>
-    <t>elerarenovaveis/Development/odata/QueueDefinitions</t>
-  </si>
-  <si>
-    <t>elerarenovaveis/Development/odata/QueueItems?$top={0}&amp;$filter=QueueDefinitionId eq {1} and (Status eq 'New' or Status eq 'Successful' or Status eq 'Failed')&amp;$orderby=StartProcessing desc&amp;$skip={2}</t>
-  </si>
-  <si>
     <t>MailParameters</t>
   </si>
   <si>
     <t>MailSender</t>
   </si>
   <si>
-    <t>svcRobo1Qa@elera.com</t>
-  </si>
-  <si>
     <t>MailSubject</t>
   </si>
   <si>
@@ -208,13 +199,22 @@
   </si>
   <si>
     <t>Empresa,CNPJ,Nível,Certidão,Data de Validade,Status,Etapa,Início</t>
+  </si>
+  <si>
+    <t>svcRobo1Prod@elera.com</t>
+  </si>
+  <si>
+    <t>elerarenovaveis/Production/odata/QueueDefinitions</t>
+  </si>
+  <si>
+    <t>elerarenovaveis/Production/odata/QueueItems?$top={0}&amp;$filter=QueueDefinitionId eq {1} and (Status eq 'New' or Status eq 'Successful' or Status eq 'Failed')&amp;$orderby=StartProcessing desc&amp;$skip={2}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -238,12 +238,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,9 +256,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -285,12 +278,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -695,7 +685,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -703,7 +693,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -716,7 +706,7 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>37</v>
@@ -748,18 +738,18 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1746,11 +1736,8 @@
     <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{4B66FB0A-7E6B-4D6F-8868-59C62E7B9350}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Calibri"&amp;11&amp;K000000_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000Pública</oddFooter>
   </headerFooter>
@@ -2875,7 +2862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2949,10 +2936,10 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>